<commit_message>
NDAcsv_to_jsonld.py is still in progress
</commit_message>
<xml_diff>
--- a/utils/BIDS_TERMS_20191122.xlsx
+++ b/utils/BIDS_TERMS_20191122.xlsx
@@ -1,31 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dbkeator/Documents/Coding/terms/utils/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC6BEA5-F4F7-8A4F-9DBA-DA7516801D4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="20225"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="76800" windowHeight="30560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="240" yWindow="240" windowWidth="38160" windowHeight="21200"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="B1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -7578,8 +7577,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="34">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="34" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -7938,12 +7937,9 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -7951,7 +7947,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8166,15 +8165,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A133" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F158" sqref="F158"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="37" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" customWidth="1"/>
@@ -8189,7 +8188,7 @@
     <col min="11" max="30" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="17">
+    <row r="1" spans="1:30">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8239,7 +8238,7 @@
       <c r="AC1" s="7"/>
       <c r="AD1" s="7"/>
     </row>
-    <row r="2" spans="1:30" ht="68">
+    <row r="2" spans="1:30" ht="60">
       <c r="A2" s="8" t="s">
         <v>9</v>
       </c>
@@ -8269,7 +8268,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="17">
+    <row r="3" spans="1:30">
       <c r="A3" s="12" t="s">
         <v>18</v>
       </c>
@@ -8297,7 +8296,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:30" ht="51">
+    <row r="4" spans="1:30" ht="45">
       <c r="A4" s="8" t="s">
         <v>22</v>
       </c>
@@ -8325,7 +8324,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="51">
+    <row r="5" spans="1:30" ht="45">
       <c r="A5" s="15" t="s">
         <v>26</v>
       </c>
@@ -8353,7 +8352,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="102">
+    <row r="6" spans="1:30" ht="90">
       <c r="A6" s="4"/>
       <c r="B6" s="5"/>
       <c r="C6" s="9" t="s">
@@ -8379,7 +8378,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="51">
+    <row r="7" spans="1:30" ht="45">
       <c r="A7" s="4"/>
       <c r="B7" s="5"/>
       <c r="C7" s="9" t="s">
@@ -8405,7 +8404,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:30" ht="17">
+    <row r="8" spans="1:30">
       <c r="A8" s="4"/>
       <c r="B8" s="5"/>
       <c r="C8" s="9" t="s">
@@ -8431,7 +8430,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:30" ht="51">
+    <row r="9" spans="1:30" ht="45">
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
       <c r="C9" s="9" t="s">
@@ -8457,7 +8456,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="51">
+    <row r="10" spans="1:30" ht="45">
       <c r="A10" s="4"/>
       <c r="B10" s="16"/>
       <c r="C10" s="9" t="s">
@@ -8483,13 +8482,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:30" ht="16">
+    <row r="11" spans="1:30">
       <c r="B11" s="17"/>
       <c r="C11" s="18"/>
       <c r="D11" s="18"/>
       <c r="F11" s="19"/>
     </row>
-    <row r="12" spans="1:30" ht="17">
+    <row r="12" spans="1:30">
       <c r="A12" s="20"/>
       <c r="B12" s="21"/>
       <c r="C12" s="21"/>
@@ -8501,7 +8500,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:30" ht="35">
+    <row r="13" spans="1:30" ht="31">
       <c r="A13" s="4"/>
       <c r="B13" s="9" t="s">
         <v>47</v>
@@ -8524,7 +8523,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:30" ht="52">
+    <row r="14" spans="1:30" ht="46">
       <c r="A14" s="15" t="s">
         <v>53</v>
       </c>
@@ -8549,7 +8548,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:30" ht="86">
+    <row r="15" spans="1:30" ht="76">
       <c r="A15" s="4"/>
       <c r="B15" s="9" t="s">
         <v>57</v>
@@ -8572,7 +8571,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:30" ht="35">
+    <row r="16" spans="1:30" ht="31">
       <c r="A16" s="4"/>
       <c r="B16" s="9" t="s">
         <v>60</v>
@@ -8595,7 +8594,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="69">
+    <row r="17" spans="1:10" ht="61">
       <c r="A17" s="15" t="s">
         <v>63</v>
       </c>
@@ -8620,7 +8619,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="52">
+    <row r="18" spans="1:10" ht="46">
       <c r="A18" s="4"/>
       <c r="B18" s="9" t="s">
         <v>67</v>
@@ -8643,7 +8642,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="35">
+    <row r="19" spans="1:10" ht="31">
       <c r="A19" s="4"/>
       <c r="B19" s="9" t="s">
         <v>70</v>
@@ -8666,7 +8665,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="69">
+    <row r="20" spans="1:10" ht="61">
       <c r="A20" s="15" t="s">
         <v>73</v>
       </c>
@@ -9655,10 +9654,10 @@
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
-      <c r="E72" s="67" t="s">
+      <c r="E72" s="66" t="s">
         <v>209</v>
       </c>
-      <c r="F72" s="68" t="s">
+      <c r="F72" s="67" t="s">
         <v>210</v>
       </c>
       <c r="G72" s="4" t="s">
@@ -9670,8 +9669,8 @@
       <c r="B73" s="5"/>
       <c r="C73" s="5"/>
       <c r="D73" s="5"/>
-      <c r="E73" s="63"/>
-      <c r="F73" s="63"/>
+      <c r="E73" s="64"/>
+      <c r="F73" s="64"/>
       <c r="G73" s="10" t="s">
         <v>212</v>
       </c>
@@ -9685,8 +9684,8 @@
       <c r="D74" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="E74" s="63"/>
-      <c r="F74" s="63"/>
+      <c r="E74" s="64"/>
+      <c r="F74" s="64"/>
       <c r="G74" s="10" t="s">
         <v>215</v>
       </c>
@@ -10982,7 +10981,7 @@
       <c r="E158" s="4" t="s">
         <v>409</v>
       </c>
-      <c r="F158" s="69" t="s">
+      <c r="F158" s="62" t="s">
         <v>410</v>
       </c>
       <c r="G158" s="10" t="s">
@@ -15923,29 +15922,29 @@
       <c r="E478" s="11" t="s">
         <v>903</v>
       </c>
-      <c r="F478" s="66" t="s">
+      <c r="F478" s="65" t="s">
         <v>904</v>
       </c>
-      <c r="G478" s="62" t="s">
+      <c r="G478" s="63" t="s">
         <v>905</v>
       </c>
-      <c r="H478" s="62"/>
-      <c r="I478" s="62" t="s">
+      <c r="H478" s="63"/>
+      <c r="I478" s="63" t="s">
         <v>905</v>
       </c>
-      <c r="J478" s="62" t="s">
+      <c r="J478" s="63" t="s">
         <v>905</v>
       </c>
-      <c r="K478" s="62" t="s">
+      <c r="K478" s="63" t="s">
         <v>905</v>
       </c>
-      <c r="L478" s="62"/>
-      <c r="M478" s="62"/>
-      <c r="N478" s="62"/>
-      <c r="O478" s="62"/>
-      <c r="P478" s="62"/>
-      <c r="Q478" s="62"/>
-      <c r="R478" s="62"/>
+      <c r="L478" s="63"/>
+      <c r="M478" s="63"/>
+      <c r="N478" s="63"/>
+      <c r="O478" s="63"/>
+      <c r="P478" s="63"/>
+      <c r="Q478" s="63"/>
+      <c r="R478" s="63"/>
     </row>
     <row r="479" spans="1:30" ht="15.75" customHeight="1">
       <c r="B479" s="17"/>
@@ -15954,19 +15953,19 @@
       <c r="E479" s="11" t="s">
         <v>906</v>
       </c>
-      <c r="F479" s="63"/>
-      <c r="G479" s="63"/>
-      <c r="H479" s="63"/>
-      <c r="I479" s="63"/>
-      <c r="J479" s="63"/>
-      <c r="K479" s="63"/>
-      <c r="L479" s="63"/>
-      <c r="M479" s="63"/>
-      <c r="N479" s="63"/>
-      <c r="O479" s="63"/>
-      <c r="P479" s="63"/>
-      <c r="Q479" s="63"/>
-      <c r="R479" s="63"/>
+      <c r="F479" s="64"/>
+      <c r="G479" s="64"/>
+      <c r="H479" s="64"/>
+      <c r="I479" s="64"/>
+      <c r="J479" s="64"/>
+      <c r="K479" s="64"/>
+      <c r="L479" s="64"/>
+      <c r="M479" s="64"/>
+      <c r="N479" s="64"/>
+      <c r="O479" s="64"/>
+      <c r="P479" s="64"/>
+      <c r="Q479" s="64"/>
+      <c r="R479" s="64"/>
     </row>
     <row r="480" spans="1:30" ht="15.75" customHeight="1">
       <c r="B480" s="17"/>
@@ -15975,31 +15974,31 @@
       <c r="E480" s="11" t="s">
         <v>903</v>
       </c>
-      <c r="F480" s="66" t="s">
+      <c r="F480" s="65" t="s">
         <v>904</v>
       </c>
-      <c r="G480" s="62" t="s">
+      <c r="G480" s="63" t="s">
         <v>905</v>
       </c>
-      <c r="H480" s="62"/>
-      <c r="I480" s="62" t="s">
+      <c r="H480" s="63"/>
+      <c r="I480" s="63" t="s">
         <v>905</v>
       </c>
-      <c r="J480" s="62" t="s">
+      <c r="J480" s="63" t="s">
         <v>905</v>
       </c>
-      <c r="K480" s="62" t="s">
+      <c r="K480" s="63" t="s">
         <v>905</v>
       </c>
-      <c r="L480" s="62"/>
-      <c r="M480" s="62"/>
-      <c r="N480" s="62" t="s">
+      <c r="L480" s="63"/>
+      <c r="M480" s="63"/>
+      <c r="N480" s="63" t="s">
         <v>905</v>
       </c>
-      <c r="O480" s="62"/>
-      <c r="P480" s="62"/>
-      <c r="Q480" s="62"/>
-      <c r="R480" s="62"/>
+      <c r="O480" s="63"/>
+      <c r="P480" s="63"/>
+      <c r="Q480" s="63"/>
+      <c r="R480" s="63"/>
     </row>
     <row r="481" spans="1:18" ht="15.75" customHeight="1">
       <c r="B481" s="17"/>
@@ -16008,19 +16007,19 @@
       <c r="E481" s="11" t="s">
         <v>907</v>
       </c>
-      <c r="F481" s="63"/>
-      <c r="G481" s="63"/>
-      <c r="H481" s="63"/>
-      <c r="I481" s="63"/>
-      <c r="J481" s="63"/>
-      <c r="K481" s="63"/>
-      <c r="L481" s="63"/>
-      <c r="M481" s="63"/>
-      <c r="N481" s="63"/>
-      <c r="O481" s="63"/>
-      <c r="P481" s="63"/>
-      <c r="Q481" s="63"/>
-      <c r="R481" s="63"/>
+      <c r="F481" s="64"/>
+      <c r="G481" s="64"/>
+      <c r="H481" s="64"/>
+      <c r="I481" s="64"/>
+      <c r="J481" s="64"/>
+      <c r="K481" s="64"/>
+      <c r="L481" s="64"/>
+      <c r="M481" s="64"/>
+      <c r="N481" s="64"/>
+      <c r="O481" s="64"/>
+      <c r="P481" s="64"/>
+      <c r="Q481" s="64"/>
+      <c r="R481" s="64"/>
     </row>
     <row r="482" spans="1:18" ht="15.75" customHeight="1">
       <c r="A482" s="29" t="s">
@@ -16032,37 +16031,37 @@
       <c r="E482" s="11" t="s">
         <v>909</v>
       </c>
-      <c r="F482" s="66" t="s">
+      <c r="F482" s="65" t="s">
         <v>904</v>
       </c>
-      <c r="G482" s="62" t="s">
+      <c r="G482" s="63" t="s">
         <v>905</v>
       </c>
-      <c r="H482" s="62" t="s">
+      <c r="H482" s="63" t="s">
         <v>904</v>
       </c>
-      <c r="I482" s="62" t="s">
+      <c r="I482" s="63" t="s">
         <v>905</v>
       </c>
-      <c r="J482" s="62" t="s">
+      <c r="J482" s="63" t="s">
         <v>905</v>
       </c>
-      <c r="K482" s="62" t="s">
+      <c r="K482" s="63" t="s">
         <v>905</v>
       </c>
-      <c r="L482" s="62" t="s">
+      <c r="L482" s="63" t="s">
         <v>905</v>
       </c>
-      <c r="M482" s="62" t="s">
+      <c r="M482" s="63" t="s">
         <v>905</v>
       </c>
-      <c r="N482" s="62"/>
-      <c r="O482" s="62" t="s">
+      <c r="N482" s="63"/>
+      <c r="O482" s="63" t="s">
         <v>905</v>
       </c>
-      <c r="P482" s="62"/>
-      <c r="Q482" s="62"/>
-      <c r="R482" s="62"/>
+      <c r="P482" s="63"/>
+      <c r="Q482" s="63"/>
+      <c r="R482" s="63"/>
     </row>
     <row r="483" spans="1:18" ht="15.75" customHeight="1">
       <c r="B483" s="17"/>
@@ -16071,19 +16070,19 @@
       <c r="E483" s="11" t="s">
         <v>910</v>
       </c>
-      <c r="F483" s="63"/>
-      <c r="G483" s="63"/>
-      <c r="H483" s="63"/>
-      <c r="I483" s="63"/>
-      <c r="J483" s="63"/>
-      <c r="K483" s="63"/>
-      <c r="L483" s="63"/>
-      <c r="M483" s="63"/>
-      <c r="N483" s="63"/>
-      <c r="O483" s="63"/>
-      <c r="P483" s="63"/>
-      <c r="Q483" s="63"/>
-      <c r="R483" s="63"/>
+      <c r="F483" s="64"/>
+      <c r="G483" s="64"/>
+      <c r="H483" s="64"/>
+      <c r="I483" s="64"/>
+      <c r="J483" s="64"/>
+      <c r="K483" s="64"/>
+      <c r="L483" s="64"/>
+      <c r="M483" s="64"/>
+      <c r="N483" s="64"/>
+      <c r="O483" s="64"/>
+      <c r="P483" s="64"/>
+      <c r="Q483" s="64"/>
+      <c r="R483" s="64"/>
     </row>
     <row r="484" spans="1:18" ht="15.75" customHeight="1">
       <c r="B484" s="17"/>
@@ -16092,35 +16091,35 @@
       <c r="E484" s="11" t="s">
         <v>909</v>
       </c>
-      <c r="F484" s="66" t="s">
+      <c r="F484" s="65" t="s">
         <v>904</v>
       </c>
-      <c r="G484" s="62" t="s">
+      <c r="G484" s="63" t="s">
         <v>905</v>
       </c>
-      <c r="H484" s="62" t="s">
+      <c r="H484" s="63" t="s">
         <v>904</v>
       </c>
-      <c r="I484" s="62" t="s">
+      <c r="I484" s="63" t="s">
         <v>905</v>
       </c>
-      <c r="J484" s="62"/>
-      <c r="K484" s="62" t="s">
+      <c r="J484" s="63"/>
+      <c r="K484" s="63" t="s">
         <v>905</v>
       </c>
-      <c r="L484" s="62"/>
-      <c r="M484" s="62" t="s">
+      <c r="L484" s="63"/>
+      <c r="M484" s="63" t="s">
         <v>905</v>
       </c>
-      <c r="N484" s="62"/>
-      <c r="O484" s="62"/>
-      <c r="P484" s="62" t="s">
+      <c r="N484" s="63"/>
+      <c r="O484" s="63"/>
+      <c r="P484" s="63" t="s">
         <v>905</v>
       </c>
-      <c r="Q484" s="62" t="s">
+      <c r="Q484" s="63" t="s">
         <v>905</v>
       </c>
-      <c r="R484" s="62"/>
+      <c r="R484" s="63"/>
     </row>
     <row r="485" spans="1:18" ht="15.75" customHeight="1">
       <c r="B485" s="17"/>
@@ -16129,19 +16128,19 @@
       <c r="E485" s="11" t="s">
         <v>911</v>
       </c>
-      <c r="F485" s="63"/>
-      <c r="G485" s="63"/>
-      <c r="H485" s="63"/>
-      <c r="I485" s="63"/>
-      <c r="J485" s="63"/>
-      <c r="K485" s="63"/>
-      <c r="L485" s="63"/>
-      <c r="M485" s="63"/>
-      <c r="N485" s="63"/>
-      <c r="O485" s="63"/>
-      <c r="P485" s="63"/>
-      <c r="Q485" s="63"/>
-      <c r="R485" s="63"/>
+      <c r="F485" s="64"/>
+      <c r="G485" s="64"/>
+      <c r="H485" s="64"/>
+      <c r="I485" s="64"/>
+      <c r="J485" s="64"/>
+      <c r="K485" s="64"/>
+      <c r="L485" s="64"/>
+      <c r="M485" s="64"/>
+      <c r="N485" s="64"/>
+      <c r="O485" s="64"/>
+      <c r="P485" s="64"/>
+      <c r="Q485" s="64"/>
+      <c r="R485" s="64"/>
     </row>
     <row r="486" spans="1:18" ht="15.75" customHeight="1">
       <c r="A486" s="29" t="s">
@@ -16153,29 +16152,29 @@
       <c r="E486" s="11" t="s">
         <v>913</v>
       </c>
-      <c r="F486" s="66" t="s">
+      <c r="F486" s="65" t="s">
         <v>904</v>
       </c>
-      <c r="G486" s="62" t="s">
+      <c r="G486" s="63" t="s">
         <v>905</v>
       </c>
-      <c r="H486" s="62"/>
-      <c r="I486" s="62" t="s">
+      <c r="H486" s="63"/>
+      <c r="I486" s="63" t="s">
         <v>905</v>
       </c>
-      <c r="J486" s="62"/>
-      <c r="K486" s="62"/>
-      <c r="L486" s="62" t="s">
+      <c r="J486" s="63"/>
+      <c r="K486" s="63"/>
+      <c r="L486" s="63" t="s">
         <v>905</v>
       </c>
-      <c r="M486" s="62" t="s">
+      <c r="M486" s="63" t="s">
         <v>905</v>
       </c>
-      <c r="N486" s="62"/>
-      <c r="O486" s="62"/>
-      <c r="P486" s="62"/>
-      <c r="Q486" s="62"/>
-      <c r="R486" s="62"/>
+      <c r="N486" s="63"/>
+      <c r="O486" s="63"/>
+      <c r="P486" s="63"/>
+      <c r="Q486" s="63"/>
+      <c r="R486" s="63"/>
     </row>
     <row r="487" spans="1:18" ht="15.75" customHeight="1">
       <c r="B487" s="17"/>
@@ -16184,19 +16183,19 @@
       <c r="E487" s="11" t="s">
         <v>914</v>
       </c>
-      <c r="F487" s="63"/>
-      <c r="G487" s="63"/>
-      <c r="H487" s="63"/>
-      <c r="I487" s="63"/>
-      <c r="J487" s="63"/>
-      <c r="K487" s="63"/>
-      <c r="L487" s="63"/>
-      <c r="M487" s="63"/>
-      <c r="N487" s="63"/>
-      <c r="O487" s="63"/>
-      <c r="P487" s="63"/>
-      <c r="Q487" s="63"/>
-      <c r="R487" s="63"/>
+      <c r="F487" s="64"/>
+      <c r="G487" s="64"/>
+      <c r="H487" s="64"/>
+      <c r="I487" s="64"/>
+      <c r="J487" s="64"/>
+      <c r="K487" s="64"/>
+      <c r="L487" s="64"/>
+      <c r="M487" s="64"/>
+      <c r="N487" s="64"/>
+      <c r="O487" s="64"/>
+      <c r="P487" s="64"/>
+      <c r="Q487" s="64"/>
+      <c r="R487" s="64"/>
     </row>
     <row r="488" spans="1:18" ht="15.75" customHeight="1">
       <c r="B488" s="17"/>
@@ -16205,27 +16204,27 @@
       <c r="E488" s="11" t="s">
         <v>915</v>
       </c>
-      <c r="F488" s="66" t="s">
+      <c r="F488" s="65" t="s">
         <v>904</v>
       </c>
-      <c r="G488" s="62" t="s">
+      <c r="G488" s="63" t="s">
         <v>905</v>
       </c>
-      <c r="H488" s="62"/>
-      <c r="I488" s="62" t="s">
+      <c r="H488" s="63"/>
+      <c r="I488" s="63" t="s">
         <v>905</v>
       </c>
-      <c r="J488" s="62"/>
-      <c r="K488" s="62"/>
-      <c r="L488" s="62"/>
-      <c r="M488" s="62" t="s">
+      <c r="J488" s="63"/>
+      <c r="K488" s="63"/>
+      <c r="L488" s="63"/>
+      <c r="M488" s="63" t="s">
         <v>905</v>
       </c>
-      <c r="N488" s="62"/>
-      <c r="O488" s="62"/>
-      <c r="P488" s="62"/>
-      <c r="Q488" s="62"/>
-      <c r="R488" s="62"/>
+      <c r="N488" s="63"/>
+      <c r="O488" s="63"/>
+      <c r="P488" s="63"/>
+      <c r="Q488" s="63"/>
+      <c r="R488" s="63"/>
     </row>
     <row r="489" spans="1:18" ht="15.75" customHeight="1">
       <c r="B489" s="17"/>
@@ -16234,19 +16233,19 @@
       <c r="E489" s="11" t="s">
         <v>916</v>
       </c>
-      <c r="F489" s="63"/>
-      <c r="G489" s="63"/>
-      <c r="H489" s="63"/>
-      <c r="I489" s="63"/>
-      <c r="J489" s="63"/>
-      <c r="K489" s="63"/>
-      <c r="L489" s="63"/>
-      <c r="M489" s="63"/>
-      <c r="N489" s="63"/>
-      <c r="O489" s="63"/>
-      <c r="P489" s="63"/>
-      <c r="Q489" s="63"/>
-      <c r="R489" s="63"/>
+      <c r="F489" s="64"/>
+      <c r="G489" s="64"/>
+      <c r="H489" s="64"/>
+      <c r="I489" s="64"/>
+      <c r="J489" s="64"/>
+      <c r="K489" s="64"/>
+      <c r="L489" s="64"/>
+      <c r="M489" s="64"/>
+      <c r="N489" s="64"/>
+      <c r="O489" s="64"/>
+      <c r="P489" s="64"/>
+      <c r="Q489" s="64"/>
+      <c r="R489" s="64"/>
     </row>
     <row r="490" spans="1:18" ht="15.75" customHeight="1">
       <c r="B490" s="17"/>
@@ -16255,31 +16254,31 @@
       <c r="E490" s="11" t="s">
         <v>915</v>
       </c>
-      <c r="F490" s="66" t="s">
+      <c r="F490" s="65" t="s">
         <v>904</v>
       </c>
-      <c r="G490" s="62" t="s">
+      <c r="G490" s="63" t="s">
         <v>905</v>
       </c>
-      <c r="H490" s="62"/>
-      <c r="I490" s="62" t="s">
+      <c r="H490" s="63"/>
+      <c r="I490" s="63" t="s">
         <v>905</v>
       </c>
-      <c r="J490" s="62" t="s">
+      <c r="J490" s="63" t="s">
         <v>905</v>
       </c>
-      <c r="K490" s="62"/>
-      <c r="L490" s="62" t="s">
+      <c r="K490" s="63"/>
+      <c r="L490" s="63" t="s">
         <v>904</v>
       </c>
-      <c r="M490" s="62" t="s">
+      <c r="M490" s="63" t="s">
         <v>905</v>
       </c>
-      <c r="N490" s="62"/>
-      <c r="O490" s="62"/>
-      <c r="P490" s="62"/>
-      <c r="Q490" s="62"/>
-      <c r="R490" s="62"/>
+      <c r="N490" s="63"/>
+      <c r="O490" s="63"/>
+      <c r="P490" s="63"/>
+      <c r="Q490" s="63"/>
+      <c r="R490" s="63"/>
     </row>
     <row r="491" spans="1:18" ht="15.75" customHeight="1">
       <c r="B491" s="17"/>
@@ -16288,19 +16287,19 @@
       <c r="E491" s="11" t="s">
         <v>917</v>
       </c>
-      <c r="F491" s="63"/>
-      <c r="G491" s="63"/>
-      <c r="H491" s="63"/>
-      <c r="I491" s="63"/>
-      <c r="J491" s="63"/>
-      <c r="K491" s="63"/>
-      <c r="L491" s="63"/>
-      <c r="M491" s="63"/>
-      <c r="N491" s="63"/>
-      <c r="O491" s="63"/>
-      <c r="P491" s="63"/>
-      <c r="Q491" s="63"/>
-      <c r="R491" s="63"/>
+      <c r="F491" s="64"/>
+      <c r="G491" s="64"/>
+      <c r="H491" s="64"/>
+      <c r="I491" s="64"/>
+      <c r="J491" s="64"/>
+      <c r="K491" s="64"/>
+      <c r="L491" s="64"/>
+      <c r="M491" s="64"/>
+      <c r="N491" s="64"/>
+      <c r="O491" s="64"/>
+      <c r="P491" s="64"/>
+      <c r="Q491" s="64"/>
+      <c r="R491" s="64"/>
     </row>
     <row r="492" spans="1:18" ht="15.75" customHeight="1">
       <c r="B492" s="17"/>
@@ -16309,25 +16308,25 @@
       <c r="E492" s="11" t="s">
         <v>918</v>
       </c>
-      <c r="F492" s="66" t="s">
+      <c r="F492" s="65" t="s">
         <v>904</v>
       </c>
-      <c r="G492" s="62" t="s">
+      <c r="G492" s="63" t="s">
         <v>905</v>
       </c>
-      <c r="H492" s="62" t="s">
+      <c r="H492" s="63" t="s">
         <v>904</v>
       </c>
-      <c r="I492" s="62"/>
-      <c r="J492" s="62"/>
-      <c r="K492" s="62"/>
-      <c r="L492" s="62"/>
-      <c r="M492" s="62"/>
-      <c r="N492" s="62"/>
-      <c r="O492" s="62"/>
-      <c r="P492" s="62"/>
-      <c r="Q492" s="62"/>
-      <c r="R492" s="62"/>
+      <c r="I492" s="63"/>
+      <c r="J492" s="63"/>
+      <c r="K492" s="63"/>
+      <c r="L492" s="63"/>
+      <c r="M492" s="63"/>
+      <c r="N492" s="63"/>
+      <c r="O492" s="63"/>
+      <c r="P492" s="63"/>
+      <c r="Q492" s="63"/>
+      <c r="R492" s="63"/>
     </row>
     <row r="493" spans="1:18" ht="15.75" customHeight="1">
       <c r="B493" s="17"/>
@@ -16336,19 +16335,19 @@
       <c r="E493" s="11" t="s">
         <v>919</v>
       </c>
-      <c r="F493" s="63"/>
-      <c r="G493" s="63"/>
-      <c r="H493" s="63"/>
-      <c r="I493" s="63"/>
-      <c r="J493" s="63"/>
-      <c r="K493" s="63"/>
-      <c r="L493" s="63"/>
-      <c r="M493" s="63"/>
-      <c r="N493" s="63"/>
-      <c r="O493" s="63"/>
-      <c r="P493" s="63"/>
-      <c r="Q493" s="63"/>
-      <c r="R493" s="63"/>
+      <c r="F493" s="64"/>
+      <c r="G493" s="64"/>
+      <c r="H493" s="64"/>
+      <c r="I493" s="64"/>
+      <c r="J493" s="64"/>
+      <c r="K493" s="64"/>
+      <c r="L493" s="64"/>
+      <c r="M493" s="64"/>
+      <c r="N493" s="64"/>
+      <c r="O493" s="64"/>
+      <c r="P493" s="64"/>
+      <c r="Q493" s="64"/>
+      <c r="R493" s="64"/>
     </row>
     <row r="494" spans="1:18" ht="15.75" customHeight="1">
       <c r="B494" s="17"/>
@@ -16429,27 +16428,27 @@
       <c r="E497" s="11" t="s">
         <v>923</v>
       </c>
-      <c r="F497" s="66" t="s">
+      <c r="F497" s="65" t="s">
         <v>904</v>
       </c>
-      <c r="G497" s="62" t="s">
+      <c r="G497" s="63" t="s">
         <v>905</v>
       </c>
-      <c r="H497" s="62" t="s">
+      <c r="H497" s="63" t="s">
         <v>904</v>
       </c>
-      <c r="I497" s="62"/>
-      <c r="J497" s="62"/>
-      <c r="K497" s="62"/>
-      <c r="L497" s="62"/>
-      <c r="M497" s="62" t="s">
+      <c r="I497" s="63"/>
+      <c r="J497" s="63"/>
+      <c r="K497" s="63"/>
+      <c r="L497" s="63"/>
+      <c r="M497" s="63" t="s">
         <v>905</v>
       </c>
-      <c r="N497" s="62"/>
-      <c r="O497" s="62"/>
-      <c r="P497" s="62"/>
-      <c r="Q497" s="62"/>
-      <c r="R497" s="62"/>
+      <c r="N497" s="63"/>
+      <c r="O497" s="63"/>
+      <c r="P497" s="63"/>
+      <c r="Q497" s="63"/>
+      <c r="R497" s="63"/>
     </row>
     <row r="498" spans="1:30" ht="15.75" customHeight="1">
       <c r="B498" s="17"/>
@@ -16458,19 +16457,19 @@
       <c r="E498" s="11" t="s">
         <v>924</v>
       </c>
-      <c r="F498" s="63"/>
-      <c r="G498" s="63"/>
-      <c r="H498" s="63"/>
-      <c r="I498" s="63"/>
-      <c r="J498" s="63"/>
-      <c r="K498" s="63"/>
-      <c r="L498" s="63"/>
-      <c r="M498" s="63"/>
-      <c r="N498" s="63"/>
-      <c r="O498" s="63"/>
-      <c r="P498" s="63"/>
-      <c r="Q498" s="63"/>
-      <c r="R498" s="63"/>
+      <c r="F498" s="64"/>
+      <c r="G498" s="64"/>
+      <c r="H498" s="64"/>
+      <c r="I498" s="64"/>
+      <c r="J498" s="64"/>
+      <c r="K498" s="64"/>
+      <c r="L498" s="64"/>
+      <c r="M498" s="64"/>
+      <c r="N498" s="64"/>
+      <c r="O498" s="64"/>
+      <c r="P498" s="64"/>
+      <c r="Q498" s="64"/>
+      <c r="R498" s="64"/>
     </row>
     <row r="499" spans="1:30" ht="15.75" customHeight="1">
       <c r="B499" s="17"/>
@@ -16479,25 +16478,25 @@
       <c r="E499" s="11" t="s">
         <v>925</v>
       </c>
-      <c r="F499" s="66" t="s">
+      <c r="F499" s="65" t="s">
         <v>904</v>
       </c>
-      <c r="G499" s="62" t="s">
+      <c r="G499" s="63" t="s">
         <v>905</v>
       </c>
-      <c r="H499" s="62"/>
-      <c r="I499" s="62" t="s">
+      <c r="H499" s="63"/>
+      <c r="I499" s="63" t="s">
         <v>905</v>
       </c>
-      <c r="J499" s="62"/>
-      <c r="K499" s="62"/>
-      <c r="L499" s="62"/>
-      <c r="M499" s="62"/>
-      <c r="N499" s="62"/>
-      <c r="O499" s="62"/>
-      <c r="P499" s="62"/>
-      <c r="Q499" s="62"/>
-      <c r="R499" s="62" t="s">
+      <c r="J499" s="63"/>
+      <c r="K499" s="63"/>
+      <c r="L499" s="63"/>
+      <c r="M499" s="63"/>
+      <c r="N499" s="63"/>
+      <c r="O499" s="63"/>
+      <c r="P499" s="63"/>
+      <c r="Q499" s="63"/>
+      <c r="R499" s="63" t="s">
         <v>905</v>
       </c>
     </row>
@@ -16508,19 +16507,19 @@
       <c r="E500" s="11" t="s">
         <v>926</v>
       </c>
-      <c r="F500" s="63"/>
-      <c r="G500" s="63"/>
-      <c r="H500" s="63"/>
-      <c r="I500" s="63"/>
-      <c r="J500" s="63"/>
-      <c r="K500" s="63"/>
-      <c r="L500" s="63"/>
-      <c r="M500" s="63"/>
-      <c r="N500" s="63"/>
-      <c r="O500" s="63"/>
-      <c r="P500" s="63"/>
-      <c r="Q500" s="63"/>
-      <c r="R500" s="63"/>
+      <c r="F500" s="64"/>
+      <c r="G500" s="64"/>
+      <c r="H500" s="64"/>
+      <c r="I500" s="64"/>
+      <c r="J500" s="64"/>
+      <c r="K500" s="64"/>
+      <c r="L500" s="64"/>
+      <c r="M500" s="64"/>
+      <c r="N500" s="64"/>
+      <c r="O500" s="64"/>
+      <c r="P500" s="64"/>
+      <c r="Q500" s="64"/>
+      <c r="R500" s="64"/>
     </row>
     <row r="501" spans="1:30" ht="15.75" customHeight="1">
       <c r="B501" s="17"/>
@@ -16529,27 +16528,27 @@
       <c r="E501" s="11" t="s">
         <v>927</v>
       </c>
-      <c r="F501" s="66" t="s">
+      <c r="F501" s="65" t="s">
         <v>904</v>
       </c>
-      <c r="G501" s="62" t="s">
+      <c r="G501" s="63" t="s">
         <v>905</v>
       </c>
-      <c r="H501" s="62" t="s">
+      <c r="H501" s="63" t="s">
         <v>905</v>
       </c>
-      <c r="I501" s="62" t="s">
+      <c r="I501" s="63" t="s">
         <v>905</v>
       </c>
-      <c r="J501" s="62"/>
-      <c r="K501" s="62"/>
-      <c r="L501" s="62"/>
-      <c r="M501" s="62"/>
-      <c r="N501" s="62"/>
-      <c r="O501" s="62"/>
-      <c r="P501" s="62"/>
-      <c r="Q501" s="62"/>
-      <c r="R501" s="62" t="s">
+      <c r="J501" s="63"/>
+      <c r="K501" s="63"/>
+      <c r="L501" s="63"/>
+      <c r="M501" s="63"/>
+      <c r="N501" s="63"/>
+      <c r="O501" s="63"/>
+      <c r="P501" s="63"/>
+      <c r="Q501" s="63"/>
+      <c r="R501" s="63" t="s">
         <v>905</v>
       </c>
     </row>
@@ -16560,19 +16559,19 @@
       <c r="E502" s="11" t="s">
         <v>926</v>
       </c>
-      <c r="F502" s="63"/>
-      <c r="G502" s="63"/>
-      <c r="H502" s="63"/>
-      <c r="I502" s="63"/>
-      <c r="J502" s="63"/>
-      <c r="K502" s="63"/>
-      <c r="L502" s="63"/>
-      <c r="M502" s="63"/>
-      <c r="N502" s="63"/>
-      <c r="O502" s="63"/>
-      <c r="P502" s="63"/>
-      <c r="Q502" s="63"/>
-      <c r="R502" s="63"/>
+      <c r="F502" s="64"/>
+      <c r="G502" s="64"/>
+      <c r="H502" s="64"/>
+      <c r="I502" s="64"/>
+      <c r="J502" s="64"/>
+      <c r="K502" s="64"/>
+      <c r="L502" s="64"/>
+      <c r="M502" s="64"/>
+      <c r="N502" s="64"/>
+      <c r="O502" s="64"/>
+      <c r="P502" s="64"/>
+      <c r="Q502" s="64"/>
+      <c r="R502" s="64"/>
     </row>
     <row r="503" spans="1:30" ht="15.75" customHeight="1">
       <c r="B503" s="17"/>
@@ -16581,25 +16580,25 @@
       <c r="E503" s="11" t="s">
         <v>928</v>
       </c>
-      <c r="F503" s="66" t="s">
+      <c r="F503" s="65" t="s">
         <v>904</v>
       </c>
-      <c r="G503" s="62" t="s">
+      <c r="G503" s="63" t="s">
         <v>905</v>
       </c>
-      <c r="H503" s="62"/>
-      <c r="I503" s="62" t="s">
+      <c r="H503" s="63"/>
+      <c r="I503" s="63" t="s">
         <v>905</v>
       </c>
-      <c r="J503" s="62"/>
-      <c r="K503" s="62"/>
-      <c r="L503" s="62"/>
-      <c r="M503" s="62"/>
-      <c r="N503" s="62"/>
-      <c r="O503" s="62"/>
-      <c r="P503" s="62"/>
-      <c r="Q503" s="62"/>
-      <c r="R503" s="62"/>
+      <c r="J503" s="63"/>
+      <c r="K503" s="63"/>
+      <c r="L503" s="63"/>
+      <c r="M503" s="63"/>
+      <c r="N503" s="63"/>
+      <c r="O503" s="63"/>
+      <c r="P503" s="63"/>
+      <c r="Q503" s="63"/>
+      <c r="R503" s="63"/>
     </row>
     <row r="504" spans="1:30" ht="15.75" customHeight="1">
       <c r="B504" s="17"/>
@@ -16608,19 +16607,19 @@
       <c r="E504" s="11" t="s">
         <v>924</v>
       </c>
-      <c r="F504" s="63"/>
-      <c r="G504" s="63"/>
-      <c r="H504" s="63"/>
-      <c r="I504" s="63"/>
-      <c r="J504" s="63"/>
-      <c r="K504" s="63"/>
-      <c r="L504" s="63"/>
-      <c r="M504" s="63"/>
-      <c r="N504" s="63"/>
-      <c r="O504" s="63"/>
-      <c r="P504" s="63"/>
-      <c r="Q504" s="63"/>
-      <c r="R504" s="63"/>
+      <c r="F504" s="64"/>
+      <c r="G504" s="64"/>
+      <c r="H504" s="64"/>
+      <c r="I504" s="64"/>
+      <c r="J504" s="64"/>
+      <c r="K504" s="64"/>
+      <c r="L504" s="64"/>
+      <c r="M504" s="64"/>
+      <c r="N504" s="64"/>
+      <c r="O504" s="64"/>
+      <c r="P504" s="64"/>
+      <c r="Q504" s="64"/>
+      <c r="R504" s="64"/>
     </row>
     <row r="505" spans="1:30" ht="15.75" customHeight="1">
       <c r="B505" s="17"/>
@@ -16629,25 +16628,25 @@
       <c r="E505" s="11" t="s">
         <v>929</v>
       </c>
-      <c r="F505" s="66" t="s">
+      <c r="F505" s="65" t="s">
         <v>904</v>
       </c>
-      <c r="G505" s="62" t="s">
+      <c r="G505" s="63" t="s">
         <v>905</v>
       </c>
-      <c r="H505" s="62"/>
-      <c r="I505" s="62" t="s">
+      <c r="H505" s="63"/>
+      <c r="I505" s="63" t="s">
         <v>905</v>
       </c>
-      <c r="J505" s="62"/>
-      <c r="K505" s="62"/>
-      <c r="L505" s="62"/>
-      <c r="M505" s="62"/>
-      <c r="N505" s="62"/>
-      <c r="O505" s="62"/>
-      <c r="P505" s="62"/>
-      <c r="Q505" s="62"/>
-      <c r="R505" s="62" t="s">
+      <c r="J505" s="63"/>
+      <c r="K505" s="63"/>
+      <c r="L505" s="63"/>
+      <c r="M505" s="63"/>
+      <c r="N505" s="63"/>
+      <c r="O505" s="63"/>
+      <c r="P505" s="63"/>
+      <c r="Q505" s="63"/>
+      <c r="R505" s="63" t="s">
         <v>905</v>
       </c>
     </row>
@@ -16658,19 +16657,19 @@
       <c r="E506" s="11" t="s">
         <v>930</v>
       </c>
-      <c r="F506" s="63"/>
-      <c r="G506" s="63"/>
-      <c r="H506" s="63"/>
-      <c r="I506" s="63"/>
-      <c r="J506" s="63"/>
-      <c r="K506" s="63"/>
-      <c r="L506" s="63"/>
-      <c r="M506" s="63"/>
-      <c r="N506" s="63"/>
-      <c r="O506" s="63"/>
-      <c r="P506" s="63"/>
-      <c r="Q506" s="63"/>
-      <c r="R506" s="63"/>
+      <c r="F506" s="64"/>
+      <c r="G506" s="64"/>
+      <c r="H506" s="64"/>
+      <c r="I506" s="64"/>
+      <c r="J506" s="64"/>
+      <c r="K506" s="64"/>
+      <c r="L506" s="64"/>
+      <c r="M506" s="64"/>
+      <c r="N506" s="64"/>
+      <c r="O506" s="64"/>
+      <c r="P506" s="64"/>
+      <c r="Q506" s="64"/>
+      <c r="R506" s="64"/>
     </row>
     <row r="507" spans="1:30" ht="15.75" customHeight="1">
       <c r="A507" s="50"/>
@@ -16680,13 +16679,13 @@
       <c r="E507" s="50" t="s">
         <v>931</v>
       </c>
-      <c r="F507" s="64" t="s">
+      <c r="F507" s="68" t="s">
         <v>904</v>
       </c>
-      <c r="G507" s="65" t="s">
+      <c r="G507" s="69" t="s">
         <v>905</v>
       </c>
-      <c r="H507" s="65" t="s">
+      <c r="H507" s="69" t="s">
         <v>904</v>
       </c>
     </row>
@@ -16698,9 +16697,9 @@
       <c r="E508" s="50" t="s">
         <v>924</v>
       </c>
-      <c r="F508" s="63"/>
-      <c r="G508" s="63"/>
-      <c r="H508" s="63"/>
+      <c r="F508" s="64"/>
+      <c r="G508" s="64"/>
+      <c r="H508" s="64"/>
     </row>
     <row r="509" spans="1:30" ht="15.75" customHeight="1">
       <c r="B509" s="17"/>
@@ -20714,52 +20713,97 @@
     </row>
   </sheetData>
   <mergeCells count="174">
-    <mergeCell ref="I484:I485"/>
-    <mergeCell ref="I488:I489"/>
-    <mergeCell ref="J488:J489"/>
-    <mergeCell ref="L482:L483"/>
-    <mergeCell ref="M478:M479"/>
-    <mergeCell ref="N478:N479"/>
-    <mergeCell ref="M480:M481"/>
-    <mergeCell ref="N480:N481"/>
-    <mergeCell ref="I478:I479"/>
-    <mergeCell ref="J480:J481"/>
-    <mergeCell ref="I480:I481"/>
-    <mergeCell ref="I482:I483"/>
-    <mergeCell ref="M482:M483"/>
-    <mergeCell ref="F497:F498"/>
-    <mergeCell ref="F501:F502"/>
-    <mergeCell ref="G501:G502"/>
-    <mergeCell ref="K501:K502"/>
-    <mergeCell ref="J501:J502"/>
-    <mergeCell ref="J497:J498"/>
-    <mergeCell ref="J499:J500"/>
-    <mergeCell ref="I497:I498"/>
-    <mergeCell ref="I499:I500"/>
-    <mergeCell ref="F499:F500"/>
-    <mergeCell ref="N503:N504"/>
-    <mergeCell ref="N499:N500"/>
-    <mergeCell ref="N501:N502"/>
-    <mergeCell ref="M503:M504"/>
-    <mergeCell ref="M501:M502"/>
-    <mergeCell ref="R499:R500"/>
-    <mergeCell ref="R497:R498"/>
-    <mergeCell ref="R501:R502"/>
-    <mergeCell ref="Q501:Q502"/>
-    <mergeCell ref="O503:O504"/>
-    <mergeCell ref="O501:O502"/>
-    <mergeCell ref="P503:P504"/>
-    <mergeCell ref="P501:P502"/>
-    <mergeCell ref="K499:K500"/>
-    <mergeCell ref="L501:L502"/>
-    <mergeCell ref="L499:L500"/>
-    <mergeCell ref="K503:K504"/>
-    <mergeCell ref="L503:L504"/>
-    <mergeCell ref="I503:I504"/>
-    <mergeCell ref="I501:I502"/>
-    <mergeCell ref="H503:H504"/>
-    <mergeCell ref="G503:G504"/>
-    <mergeCell ref="F503:F504"/>
+    <mergeCell ref="Q492:Q493"/>
+    <mergeCell ref="R492:R493"/>
+    <mergeCell ref="R490:R491"/>
+    <mergeCell ref="O484:O485"/>
+    <mergeCell ref="N484:N485"/>
+    <mergeCell ref="M490:M491"/>
+    <mergeCell ref="N490:N491"/>
+    <mergeCell ref="L490:L491"/>
+    <mergeCell ref="Q490:Q491"/>
+    <mergeCell ref="P492:P493"/>
+    <mergeCell ref="M484:M485"/>
+    <mergeCell ref="M486:M487"/>
+    <mergeCell ref="M488:M489"/>
+    <mergeCell ref="N488:N489"/>
+    <mergeCell ref="N486:N487"/>
+    <mergeCell ref="L478:L479"/>
+    <mergeCell ref="P486:P487"/>
+    <mergeCell ref="P490:P491"/>
+    <mergeCell ref="R480:R481"/>
+    <mergeCell ref="R482:R483"/>
+    <mergeCell ref="O478:O479"/>
+    <mergeCell ref="O482:O483"/>
+    <mergeCell ref="O480:O481"/>
+    <mergeCell ref="R486:R487"/>
+    <mergeCell ref="Q486:Q487"/>
+    <mergeCell ref="P480:P481"/>
+    <mergeCell ref="P482:P483"/>
+    <mergeCell ref="Q482:Q483"/>
+    <mergeCell ref="Q480:Q481"/>
+    <mergeCell ref="Q478:Q479"/>
+    <mergeCell ref="R488:R489"/>
+    <mergeCell ref="R484:R485"/>
+    <mergeCell ref="P484:P485"/>
+    <mergeCell ref="R478:R479"/>
+    <mergeCell ref="P478:P479"/>
+    <mergeCell ref="M492:M493"/>
+    <mergeCell ref="L488:L489"/>
+    <mergeCell ref="O497:O498"/>
+    <mergeCell ref="K505:K506"/>
+    <mergeCell ref="I505:I506"/>
+    <mergeCell ref="J505:J506"/>
+    <mergeCell ref="I486:I487"/>
+    <mergeCell ref="P488:P489"/>
+    <mergeCell ref="J486:J487"/>
+    <mergeCell ref="O486:O487"/>
+    <mergeCell ref="N492:N493"/>
+    <mergeCell ref="O492:O493"/>
+    <mergeCell ref="O490:O491"/>
+    <mergeCell ref="O488:O489"/>
+    <mergeCell ref="K497:K498"/>
+    <mergeCell ref="L497:L498"/>
+    <mergeCell ref="K486:K487"/>
+    <mergeCell ref="K490:K491"/>
+    <mergeCell ref="K488:K489"/>
+    <mergeCell ref="M497:M498"/>
+    <mergeCell ref="N497:N498"/>
+    <mergeCell ref="F507:F508"/>
+    <mergeCell ref="G507:G508"/>
+    <mergeCell ref="H507:H508"/>
+    <mergeCell ref="O505:O506"/>
+    <mergeCell ref="P505:P506"/>
+    <mergeCell ref="N505:N506"/>
+    <mergeCell ref="F505:F506"/>
+    <mergeCell ref="G505:G506"/>
+    <mergeCell ref="L505:L506"/>
+    <mergeCell ref="M505:M506"/>
+    <mergeCell ref="H505:H506"/>
+    <mergeCell ref="H492:H493"/>
+    <mergeCell ref="H490:H491"/>
+    <mergeCell ref="H478:H479"/>
+    <mergeCell ref="H486:H487"/>
+    <mergeCell ref="H480:H481"/>
+    <mergeCell ref="H482:H483"/>
+    <mergeCell ref="H488:H489"/>
+    <mergeCell ref="F478:F479"/>
+    <mergeCell ref="E72:E74"/>
+    <mergeCell ref="F72:F74"/>
+    <mergeCell ref="F488:F489"/>
+    <mergeCell ref="F486:F487"/>
+    <mergeCell ref="F482:F483"/>
+    <mergeCell ref="F484:F485"/>
+    <mergeCell ref="G488:G489"/>
+    <mergeCell ref="F492:F493"/>
+    <mergeCell ref="G492:G493"/>
+    <mergeCell ref="F490:F491"/>
+    <mergeCell ref="F480:F481"/>
+    <mergeCell ref="G478:G479"/>
+    <mergeCell ref="G480:G481"/>
+    <mergeCell ref="G482:G483"/>
+    <mergeCell ref="G486:G487"/>
+    <mergeCell ref="G490:G491"/>
     <mergeCell ref="G484:G485"/>
     <mergeCell ref="H484:H485"/>
     <mergeCell ref="I490:I491"/>
@@ -20784,68 +20828,58 @@
     <mergeCell ref="J503:J504"/>
     <mergeCell ref="Q484:Q485"/>
     <mergeCell ref="Q488:Q489"/>
-    <mergeCell ref="H492:H493"/>
-    <mergeCell ref="H490:H491"/>
-    <mergeCell ref="H478:H479"/>
-    <mergeCell ref="H486:H487"/>
-    <mergeCell ref="H480:H481"/>
-    <mergeCell ref="H482:H483"/>
-    <mergeCell ref="H488:H489"/>
-    <mergeCell ref="F478:F479"/>
-    <mergeCell ref="E72:E74"/>
-    <mergeCell ref="F72:F74"/>
-    <mergeCell ref="F488:F489"/>
-    <mergeCell ref="F486:F487"/>
-    <mergeCell ref="F482:F483"/>
-    <mergeCell ref="F484:F485"/>
-    <mergeCell ref="G488:G489"/>
-    <mergeCell ref="F492:F493"/>
-    <mergeCell ref="G492:G493"/>
-    <mergeCell ref="F490:F491"/>
-    <mergeCell ref="F480:F481"/>
-    <mergeCell ref="G478:G479"/>
-    <mergeCell ref="G480:G481"/>
-    <mergeCell ref="G482:G483"/>
-    <mergeCell ref="G486:G487"/>
-    <mergeCell ref="G490:G491"/>
-    <mergeCell ref="F507:F508"/>
-    <mergeCell ref="G507:G508"/>
-    <mergeCell ref="H507:H508"/>
-    <mergeCell ref="O505:O506"/>
-    <mergeCell ref="P505:P506"/>
-    <mergeCell ref="N505:N506"/>
-    <mergeCell ref="F505:F506"/>
-    <mergeCell ref="G505:G506"/>
-    <mergeCell ref="L505:L506"/>
-    <mergeCell ref="M505:M506"/>
-    <mergeCell ref="H505:H506"/>
+    <mergeCell ref="L501:L502"/>
+    <mergeCell ref="L499:L500"/>
+    <mergeCell ref="K503:K504"/>
+    <mergeCell ref="L503:L504"/>
+    <mergeCell ref="I503:I504"/>
+    <mergeCell ref="I501:I502"/>
+    <mergeCell ref="H503:H504"/>
+    <mergeCell ref="G503:G504"/>
+    <mergeCell ref="F503:F504"/>
+    <mergeCell ref="N503:N504"/>
+    <mergeCell ref="N499:N500"/>
+    <mergeCell ref="N501:N502"/>
+    <mergeCell ref="M503:M504"/>
+    <mergeCell ref="M501:M502"/>
+    <mergeCell ref="R499:R500"/>
+    <mergeCell ref="R497:R498"/>
+    <mergeCell ref="R501:R502"/>
+    <mergeCell ref="Q501:Q502"/>
+    <mergeCell ref="O503:O504"/>
+    <mergeCell ref="O501:O502"/>
+    <mergeCell ref="P503:P504"/>
+    <mergeCell ref="P501:P502"/>
     <mergeCell ref="Q497:Q498"/>
     <mergeCell ref="P497:P498"/>
+    <mergeCell ref="F497:F498"/>
+    <mergeCell ref="F501:F502"/>
+    <mergeCell ref="G501:G502"/>
+    <mergeCell ref="K501:K502"/>
+    <mergeCell ref="J501:J502"/>
+    <mergeCell ref="J497:J498"/>
+    <mergeCell ref="J499:J500"/>
+    <mergeCell ref="I497:I498"/>
+    <mergeCell ref="I499:I500"/>
+    <mergeCell ref="F499:F500"/>
+    <mergeCell ref="K499:K500"/>
+    <mergeCell ref="I484:I485"/>
+    <mergeCell ref="I488:I489"/>
+    <mergeCell ref="J488:J489"/>
+    <mergeCell ref="L482:L483"/>
+    <mergeCell ref="M478:M479"/>
+    <mergeCell ref="N478:N479"/>
+    <mergeCell ref="M480:M481"/>
+    <mergeCell ref="N480:N481"/>
+    <mergeCell ref="I478:I479"/>
+    <mergeCell ref="J480:J481"/>
+    <mergeCell ref="I480:I481"/>
+    <mergeCell ref="I482:I483"/>
+    <mergeCell ref="M482:M483"/>
     <mergeCell ref="L486:L487"/>
-    <mergeCell ref="M492:M493"/>
-    <mergeCell ref="L488:L489"/>
-    <mergeCell ref="O497:O498"/>
-    <mergeCell ref="K505:K506"/>
-    <mergeCell ref="I505:I506"/>
-    <mergeCell ref="J505:J506"/>
-    <mergeCell ref="I486:I487"/>
-    <mergeCell ref="P488:P489"/>
-    <mergeCell ref="J486:J487"/>
     <mergeCell ref="J478:J479"/>
     <mergeCell ref="K478:K479"/>
     <mergeCell ref="K480:K481"/>
-    <mergeCell ref="O486:O487"/>
-    <mergeCell ref="N492:N493"/>
-    <mergeCell ref="O492:O493"/>
-    <mergeCell ref="O490:O491"/>
-    <mergeCell ref="O488:O489"/>
-    <mergeCell ref="K497:K498"/>
-    <mergeCell ref="L497:L498"/>
-    <mergeCell ref="K486:K487"/>
-    <mergeCell ref="K490:K491"/>
-    <mergeCell ref="K488:K489"/>
-    <mergeCell ref="M497:M498"/>
-    <mergeCell ref="N497:N498"/>
     <mergeCell ref="K484:K485"/>
     <mergeCell ref="K482:K483"/>
     <mergeCell ref="J482:J483"/>
@@ -20853,259 +20887,228 @@
     <mergeCell ref="J484:J485"/>
     <mergeCell ref="N482:N483"/>
     <mergeCell ref="L480:L481"/>
-    <mergeCell ref="L478:L479"/>
-    <mergeCell ref="P486:P487"/>
-    <mergeCell ref="P490:P491"/>
-    <mergeCell ref="R480:R481"/>
-    <mergeCell ref="R482:R483"/>
-    <mergeCell ref="O478:O479"/>
-    <mergeCell ref="O482:O483"/>
-    <mergeCell ref="O480:O481"/>
-    <mergeCell ref="R486:R487"/>
-    <mergeCell ref="Q486:Q487"/>
-    <mergeCell ref="P480:P481"/>
-    <mergeCell ref="P482:P483"/>
-    <mergeCell ref="Q482:Q483"/>
-    <mergeCell ref="Q480:Q481"/>
-    <mergeCell ref="Q478:Q479"/>
-    <mergeCell ref="R488:R489"/>
-    <mergeCell ref="R484:R485"/>
-    <mergeCell ref="P484:P485"/>
-    <mergeCell ref="R478:R479"/>
-    <mergeCell ref="P478:P479"/>
-    <mergeCell ref="Q492:Q493"/>
-    <mergeCell ref="R492:R493"/>
-    <mergeCell ref="R490:R491"/>
-    <mergeCell ref="O484:O485"/>
-    <mergeCell ref="N484:N485"/>
-    <mergeCell ref="M490:M491"/>
-    <mergeCell ref="N490:N491"/>
-    <mergeCell ref="L490:L491"/>
-    <mergeCell ref="Q490:Q491"/>
-    <mergeCell ref="P492:P493"/>
-    <mergeCell ref="M484:M485"/>
-    <mergeCell ref="M486:M487"/>
-    <mergeCell ref="M488:M489"/>
-    <mergeCell ref="N488:N489"/>
-    <mergeCell ref="N486:N487"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="I2" r:id="rId2" location="dataset_descriptionjson" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="G3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="G4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="G5" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="G6" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="G7" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="G8" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="G9" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="G10" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="G13" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="G19" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="G20" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="G21" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="G22" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="G28" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="G37" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="G38" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="G39" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="G40" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="G41" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="G42" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="G43" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="G44" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="G47" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="G48" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="G49" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="G50" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="G51" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="G54" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="G55" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="G56" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="G58" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="G60" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="G63" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="G64" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="G65" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="F67" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="G73" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="G74" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="G94" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="G95" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="G96" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="G98" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="G99" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="G100" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="G101" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="G102" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="G104" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="G105" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="F106" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="G106" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="F107" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="G107" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="G110" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="F113" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="F114" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="G122" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="G123" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="G124" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="G125" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="G126" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="G127" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="G129" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="G130" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="G131" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="G132" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="G133" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="G134" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="G135" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="G136" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="G137" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="G138" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="G139" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="G140" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="G141" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="G142" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="G143" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
-    <hyperlink ref="G144" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
-    <hyperlink ref="G145" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="G146" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
-    <hyperlink ref="G147" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
-    <hyperlink ref="G149" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
-    <hyperlink ref="G156" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
-    <hyperlink ref="G157" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
-    <hyperlink ref="G158" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
-    <hyperlink ref="G160" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
-    <hyperlink ref="G161" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
-    <hyperlink ref="G162" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
-    <hyperlink ref="G163" r:id="rId90" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
-    <hyperlink ref="G164" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="G165" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
-    <hyperlink ref="G166" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
-    <hyperlink ref="G167" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
-    <hyperlink ref="G169" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
-    <hyperlink ref="G188" r:id="rId96" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
-    <hyperlink ref="F199" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
-    <hyperlink ref="G199" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
-    <hyperlink ref="G206" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
-    <hyperlink ref="F207" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
-    <hyperlink ref="G207" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
-    <hyperlink ref="G208" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
-    <hyperlink ref="G209" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
-    <hyperlink ref="G211" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
-    <hyperlink ref="F212" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
-    <hyperlink ref="G212" r:id="rId106" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
-    <hyperlink ref="G213" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
-    <hyperlink ref="G214" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
-    <hyperlink ref="G216" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
-    <hyperlink ref="G218" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
-    <hyperlink ref="F219" r:id="rId111" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
-    <hyperlink ref="G219" r:id="rId112" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
-    <hyperlink ref="G220" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
-    <hyperlink ref="G221" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
-    <hyperlink ref="G223" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
-    <hyperlink ref="G227" r:id="rId116" location="electroencephalography-eeg" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
-    <hyperlink ref="G238" r:id="rId117" location="electroencephalography-eeg" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
-    <hyperlink ref="G260" r:id="rId118" location="electroencephalography-eeg" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
-    <hyperlink ref="F262" r:id="rId119" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
-    <hyperlink ref="G264" r:id="rId120" location="electroencephalography-eeg" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
-    <hyperlink ref="G273" r:id="rId121" location="electroencephalography-eeg" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
-    <hyperlink ref="G290" r:id="rId122" location="electroencephalography-eeg" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
-    <hyperlink ref="G295" r:id="rId123" location="electroencephalography-eeg" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
-    <hyperlink ref="G299" r:id="rId124" location="electroencephalography-eeg" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
-    <hyperlink ref="F301" r:id="rId125" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
-    <hyperlink ref="G301" r:id="rId126" location="electroencephalography-eeg" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
-    <hyperlink ref="G305" r:id="rId127" location="electroencephalography-eeg" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
-    <hyperlink ref="G311" r:id="rId128" location="electroencephalography-eeg" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
-    <hyperlink ref="G318" r:id="rId129" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
-    <hyperlink ref="G320" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
-    <hyperlink ref="F327" r:id="rId131" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
-    <hyperlink ref="F328" r:id="rId132" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
-    <hyperlink ref="G331" r:id="rId133" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
-    <hyperlink ref="G336" r:id="rId134" xr:uid="{00000000-0004-0000-0000-000086000000}"/>
-    <hyperlink ref="G356" r:id="rId135" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
-    <hyperlink ref="G357" r:id="rId136" xr:uid="{00000000-0004-0000-0000-000088000000}"/>
-    <hyperlink ref="G359" r:id="rId137" xr:uid="{00000000-0004-0000-0000-000089000000}"/>
-    <hyperlink ref="G365" r:id="rId138" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
-    <hyperlink ref="G373" r:id="rId139" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
-    <hyperlink ref="G395" r:id="rId140" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
-    <hyperlink ref="G400" r:id="rId141" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
-    <hyperlink ref="G405" r:id="rId142" xr:uid="{00000000-0004-0000-0000-00008E000000}"/>
-    <hyperlink ref="G409" r:id="rId143" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
-    <hyperlink ref="G411" r:id="rId144" xr:uid="{00000000-0004-0000-0000-000090000000}"/>
-    <hyperlink ref="G419" r:id="rId145" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
-    <hyperlink ref="F426" r:id="rId146" xr:uid="{00000000-0004-0000-0000-000092000000}"/>
-    <hyperlink ref="G429" r:id="rId147" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
-    <hyperlink ref="G433" r:id="rId148" xr:uid="{00000000-0004-0000-0000-000094000000}"/>
-    <hyperlink ref="E438" r:id="rId149" location="bids-extension-proposals" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
-    <hyperlink ref="E440" r:id="rId150" xr:uid="{00000000-0004-0000-0000-000096000000}"/>
-    <hyperlink ref="E441" r:id="rId151" xr:uid="{00000000-0004-0000-0000-000097000000}"/>
-    <hyperlink ref="E442" r:id="rId152" xr:uid="{00000000-0004-0000-0000-000098000000}"/>
-    <hyperlink ref="E443" r:id="rId153" xr:uid="{00000000-0004-0000-0000-000099000000}"/>
-    <hyperlink ref="E444" r:id="rId154" xr:uid="{00000000-0004-0000-0000-00009A000000}"/>
-    <hyperlink ref="E445" r:id="rId155" xr:uid="{00000000-0004-0000-0000-00009B000000}"/>
-    <hyperlink ref="E446" r:id="rId156" xr:uid="{00000000-0004-0000-0000-00009C000000}"/>
-    <hyperlink ref="E447" r:id="rId157" xr:uid="{00000000-0004-0000-0000-00009D000000}"/>
-    <hyperlink ref="E448" r:id="rId158" xr:uid="{00000000-0004-0000-0000-00009E000000}"/>
-    <hyperlink ref="E449" r:id="rId159" xr:uid="{00000000-0004-0000-0000-00009F000000}"/>
-    <hyperlink ref="E450" r:id="rId160" xr:uid="{00000000-0004-0000-0000-0000A0000000}"/>
-    <hyperlink ref="E451" r:id="rId161" xr:uid="{00000000-0004-0000-0000-0000A1000000}"/>
-    <hyperlink ref="H451" r:id="rId162" xr:uid="{00000000-0004-0000-0000-0000A2000000}"/>
-    <hyperlink ref="E452" r:id="rId163" xr:uid="{00000000-0004-0000-0000-0000A3000000}"/>
-    <hyperlink ref="E453" r:id="rId164" xr:uid="{00000000-0004-0000-0000-0000A4000000}"/>
-    <hyperlink ref="H453" r:id="rId165" xr:uid="{00000000-0004-0000-0000-0000A5000000}"/>
-    <hyperlink ref="E454" r:id="rId166" xr:uid="{00000000-0004-0000-0000-0000A6000000}"/>
-    <hyperlink ref="E455" r:id="rId167" xr:uid="{00000000-0004-0000-0000-0000A7000000}"/>
-    <hyperlink ref="E456" r:id="rId168" xr:uid="{00000000-0004-0000-0000-0000A8000000}"/>
-    <hyperlink ref="E457" r:id="rId169" xr:uid="{00000000-0004-0000-0000-0000A9000000}"/>
-    <hyperlink ref="E458" r:id="rId170" xr:uid="{00000000-0004-0000-0000-0000AA000000}"/>
-    <hyperlink ref="E459" r:id="rId171" xr:uid="{00000000-0004-0000-0000-0000AB000000}"/>
-    <hyperlink ref="E460" r:id="rId172" xr:uid="{00000000-0004-0000-0000-0000AC000000}"/>
-    <hyperlink ref="E461" r:id="rId173" xr:uid="{00000000-0004-0000-0000-0000AD000000}"/>
-    <hyperlink ref="E464" r:id="rId174" xr:uid="{00000000-0004-0000-0000-0000AE000000}"/>
-    <hyperlink ref="E465" r:id="rId175" xr:uid="{00000000-0004-0000-0000-0000AF000000}"/>
-    <hyperlink ref="E466" r:id="rId176" xr:uid="{00000000-0004-0000-0000-0000B0000000}"/>
-    <hyperlink ref="E467" r:id="rId177" xr:uid="{00000000-0004-0000-0000-0000B1000000}"/>
-    <hyperlink ref="G472" r:id="rId178" xr:uid="{00000000-0004-0000-0000-0000B2000000}"/>
-    <hyperlink ref="G473" r:id="rId179" xr:uid="{00000000-0004-0000-0000-0000B3000000}"/>
-    <hyperlink ref="E546" r:id="rId180" xr:uid="{00000000-0004-0000-0000-0000B4000000}"/>
-    <hyperlink ref="E547" r:id="rId181" xr:uid="{00000000-0004-0000-0000-0000B5000000}"/>
-    <hyperlink ref="E548" r:id="rId182" xr:uid="{00000000-0004-0000-0000-0000B6000000}"/>
-    <hyperlink ref="E549" r:id="rId183" xr:uid="{00000000-0004-0000-0000-0000B7000000}"/>
-    <hyperlink ref="E550" r:id="rId184" xr:uid="{00000000-0004-0000-0000-0000B8000000}"/>
-    <hyperlink ref="E551" r:id="rId185" xr:uid="{00000000-0004-0000-0000-0000B9000000}"/>
-    <hyperlink ref="E552" r:id="rId186" xr:uid="{00000000-0004-0000-0000-0000BA000000}"/>
-    <hyperlink ref="E553" r:id="rId187" xr:uid="{00000000-0004-0000-0000-0000BB000000}"/>
-    <hyperlink ref="E554" r:id="rId188" xr:uid="{00000000-0004-0000-0000-0000BC000000}"/>
-    <hyperlink ref="E555" r:id="rId189" xr:uid="{00000000-0004-0000-0000-0000BD000000}"/>
-    <hyperlink ref="E559" r:id="rId190" xr:uid="{00000000-0004-0000-0000-0000BE000000}"/>
-    <hyperlink ref="E560" r:id="rId191" xr:uid="{00000000-0004-0000-0000-0000BF000000}"/>
-    <hyperlink ref="E561" r:id="rId192" xr:uid="{00000000-0004-0000-0000-0000C0000000}"/>
-    <hyperlink ref="E562" r:id="rId193" xr:uid="{00000000-0004-0000-0000-0000C1000000}"/>
-    <hyperlink ref="E563" r:id="rId194" xr:uid="{00000000-0004-0000-0000-0000C2000000}"/>
-    <hyperlink ref="E564" r:id="rId195" xr:uid="{00000000-0004-0000-0000-0000C3000000}"/>
-    <hyperlink ref="E565" r:id="rId196" xr:uid="{00000000-0004-0000-0000-0000C4000000}"/>
-    <hyperlink ref="E566" r:id="rId197" xr:uid="{00000000-0004-0000-0000-0000C5000000}"/>
-    <hyperlink ref="E567" r:id="rId198" xr:uid="{00000000-0004-0000-0000-0000C6000000}"/>
-    <hyperlink ref="E568" r:id="rId199" xr:uid="{00000000-0004-0000-0000-0000C7000000}"/>
-    <hyperlink ref="E572" r:id="rId200" location="ctf" xr:uid="{00000000-0004-0000-0000-0000C8000000}"/>
-    <hyperlink ref="G572" r:id="rId201" xr:uid="{00000000-0004-0000-0000-0000C9000000}"/>
-    <hyperlink ref="E573" r:id="rId202" location="neuromagelektamegin" xr:uid="{00000000-0004-0000-0000-0000CA000000}"/>
-    <hyperlink ref="G573" r:id="rId203" xr:uid="{00000000-0004-0000-0000-0000CB000000}"/>
-    <hyperlink ref="E574" r:id="rId204" location="bti4d-neuroimaging" xr:uid="{00000000-0004-0000-0000-0000CC000000}"/>
-    <hyperlink ref="G574" r:id="rId205" xr:uid="{00000000-0004-0000-0000-0000CD000000}"/>
-    <hyperlink ref="E575" r:id="rId206" location="kityokogawaricoh" xr:uid="{00000000-0004-0000-0000-0000CE000000}"/>
-    <hyperlink ref="G575" r:id="rId207" xr:uid="{00000000-0004-0000-0000-0000CF000000}"/>
-    <hyperlink ref="E576" r:id="rId208" location="kriss" xr:uid="{00000000-0004-0000-0000-0000D0000000}"/>
-    <hyperlink ref="G576" r:id="rId209" xr:uid="{00000000-0004-0000-0000-0000D1000000}"/>
-    <hyperlink ref="E577" r:id="rId210" location="itab" xr:uid="{00000000-0004-0000-0000-0000D2000000}"/>
-    <hyperlink ref="G577" r:id="rId211" xr:uid="{00000000-0004-0000-0000-0000D3000000}"/>
-    <hyperlink ref="G583" r:id="rId212" xr:uid="{00000000-0004-0000-0000-0000D4000000}"/>
-    <hyperlink ref="G587" r:id="rId213" xr:uid="{00000000-0004-0000-0000-0000D5000000}"/>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="I2" r:id="rId2" location="dataset_descriptionjson"/>
+    <hyperlink ref="G3" r:id="rId3"/>
+    <hyperlink ref="G4" r:id="rId4"/>
+    <hyperlink ref="G5" r:id="rId5"/>
+    <hyperlink ref="G6" r:id="rId6"/>
+    <hyperlink ref="G7" r:id="rId7"/>
+    <hyperlink ref="G8" r:id="rId8"/>
+    <hyperlink ref="G9" r:id="rId9"/>
+    <hyperlink ref="G10" r:id="rId10"/>
+    <hyperlink ref="G13" r:id="rId11"/>
+    <hyperlink ref="G19" r:id="rId12"/>
+    <hyperlink ref="G20" r:id="rId13"/>
+    <hyperlink ref="G21" r:id="rId14"/>
+    <hyperlink ref="G22" r:id="rId15"/>
+    <hyperlink ref="G28" r:id="rId16"/>
+    <hyperlink ref="G37" r:id="rId17"/>
+    <hyperlink ref="G38" r:id="rId18"/>
+    <hyperlink ref="G39" r:id="rId19"/>
+    <hyperlink ref="G40" r:id="rId20"/>
+    <hyperlink ref="G41" r:id="rId21"/>
+    <hyperlink ref="G42" r:id="rId22"/>
+    <hyperlink ref="G43" r:id="rId23"/>
+    <hyperlink ref="G44" r:id="rId24"/>
+    <hyperlink ref="G47" r:id="rId25"/>
+    <hyperlink ref="G48" r:id="rId26"/>
+    <hyperlink ref="G49" r:id="rId27"/>
+    <hyperlink ref="G50" r:id="rId28"/>
+    <hyperlink ref="G51" r:id="rId29"/>
+    <hyperlink ref="G54" r:id="rId30"/>
+    <hyperlink ref="G55" r:id="rId31"/>
+    <hyperlink ref="G56" r:id="rId32"/>
+    <hyperlink ref="G58" r:id="rId33"/>
+    <hyperlink ref="G60" r:id="rId34"/>
+    <hyperlink ref="G63" r:id="rId35"/>
+    <hyperlink ref="G64" r:id="rId36"/>
+    <hyperlink ref="G65" r:id="rId37"/>
+    <hyperlink ref="F67" r:id="rId38"/>
+    <hyperlink ref="G73" r:id="rId39"/>
+    <hyperlink ref="G74" r:id="rId40"/>
+    <hyperlink ref="G94" r:id="rId41"/>
+    <hyperlink ref="G95" r:id="rId42"/>
+    <hyperlink ref="G96" r:id="rId43"/>
+    <hyperlink ref="G98" r:id="rId44"/>
+    <hyperlink ref="G99" r:id="rId45"/>
+    <hyperlink ref="G100" r:id="rId46"/>
+    <hyperlink ref="G101" r:id="rId47"/>
+    <hyperlink ref="G102" r:id="rId48"/>
+    <hyperlink ref="G104" r:id="rId49"/>
+    <hyperlink ref="G105" r:id="rId50"/>
+    <hyperlink ref="F106" r:id="rId51"/>
+    <hyperlink ref="G106" r:id="rId52"/>
+    <hyperlink ref="F107" r:id="rId53"/>
+    <hyperlink ref="G107" r:id="rId54"/>
+    <hyperlink ref="G110" r:id="rId55"/>
+    <hyperlink ref="F113" r:id="rId56"/>
+    <hyperlink ref="F114" r:id="rId57"/>
+    <hyperlink ref="G122" r:id="rId58"/>
+    <hyperlink ref="G123" r:id="rId59"/>
+    <hyperlink ref="G124" r:id="rId60"/>
+    <hyperlink ref="G125" r:id="rId61"/>
+    <hyperlink ref="G126" r:id="rId62"/>
+    <hyperlink ref="G127" r:id="rId63"/>
+    <hyperlink ref="G129" r:id="rId64"/>
+    <hyperlink ref="G130" r:id="rId65"/>
+    <hyperlink ref="G131" r:id="rId66"/>
+    <hyperlink ref="G132" r:id="rId67"/>
+    <hyperlink ref="G133" r:id="rId68"/>
+    <hyperlink ref="G134" r:id="rId69"/>
+    <hyperlink ref="G135" r:id="rId70"/>
+    <hyperlink ref="G136" r:id="rId71"/>
+    <hyperlink ref="G137" r:id="rId72"/>
+    <hyperlink ref="G138" r:id="rId73"/>
+    <hyperlink ref="G139" r:id="rId74"/>
+    <hyperlink ref="G140" r:id="rId75"/>
+    <hyperlink ref="G141" r:id="rId76"/>
+    <hyperlink ref="G142" r:id="rId77"/>
+    <hyperlink ref="G143" r:id="rId78"/>
+    <hyperlink ref="G144" r:id="rId79"/>
+    <hyperlink ref="G145" r:id="rId80"/>
+    <hyperlink ref="G146" r:id="rId81"/>
+    <hyperlink ref="G147" r:id="rId82"/>
+    <hyperlink ref="G149" r:id="rId83"/>
+    <hyperlink ref="G156" r:id="rId84"/>
+    <hyperlink ref="G157" r:id="rId85"/>
+    <hyperlink ref="G158" r:id="rId86"/>
+    <hyperlink ref="G160" r:id="rId87"/>
+    <hyperlink ref="G161" r:id="rId88"/>
+    <hyperlink ref="G162" r:id="rId89"/>
+    <hyperlink ref="G163" r:id="rId90"/>
+    <hyperlink ref="G164" r:id="rId91"/>
+    <hyperlink ref="G165" r:id="rId92"/>
+    <hyperlink ref="G166" r:id="rId93"/>
+    <hyperlink ref="G167" r:id="rId94"/>
+    <hyperlink ref="G169" r:id="rId95"/>
+    <hyperlink ref="G188" r:id="rId96"/>
+    <hyperlink ref="F199" r:id="rId97"/>
+    <hyperlink ref="G199" r:id="rId98"/>
+    <hyperlink ref="G206" r:id="rId99"/>
+    <hyperlink ref="F207" r:id="rId100"/>
+    <hyperlink ref="G207" r:id="rId101"/>
+    <hyperlink ref="G208" r:id="rId102"/>
+    <hyperlink ref="G209" r:id="rId103"/>
+    <hyperlink ref="G211" r:id="rId104"/>
+    <hyperlink ref="F212" r:id="rId105"/>
+    <hyperlink ref="G212" r:id="rId106"/>
+    <hyperlink ref="G213" r:id="rId107"/>
+    <hyperlink ref="G214" r:id="rId108"/>
+    <hyperlink ref="G216" r:id="rId109"/>
+    <hyperlink ref="G218" r:id="rId110"/>
+    <hyperlink ref="F219" r:id="rId111"/>
+    <hyperlink ref="G219" r:id="rId112"/>
+    <hyperlink ref="G220" r:id="rId113"/>
+    <hyperlink ref="G221" r:id="rId114"/>
+    <hyperlink ref="G223" r:id="rId115"/>
+    <hyperlink ref="G227" r:id="rId116" location="electroencephalography-eeg"/>
+    <hyperlink ref="G238" r:id="rId117" location="electroencephalography-eeg"/>
+    <hyperlink ref="G260" r:id="rId118" location="electroencephalography-eeg"/>
+    <hyperlink ref="F262" r:id="rId119"/>
+    <hyperlink ref="G264" r:id="rId120" location="electroencephalography-eeg"/>
+    <hyperlink ref="G273" r:id="rId121" location="electroencephalography-eeg"/>
+    <hyperlink ref="G290" r:id="rId122" location="electroencephalography-eeg"/>
+    <hyperlink ref="G295" r:id="rId123" location="electroencephalography-eeg"/>
+    <hyperlink ref="G299" r:id="rId124" location="electroencephalography-eeg"/>
+    <hyperlink ref="F301" r:id="rId125"/>
+    <hyperlink ref="G301" r:id="rId126" location="electroencephalography-eeg"/>
+    <hyperlink ref="G305" r:id="rId127" location="electroencephalography-eeg"/>
+    <hyperlink ref="G311" r:id="rId128" location="electroencephalography-eeg"/>
+    <hyperlink ref="G318" r:id="rId129"/>
+    <hyperlink ref="G320" r:id="rId130"/>
+    <hyperlink ref="F327" r:id="rId131"/>
+    <hyperlink ref="F328" r:id="rId132"/>
+    <hyperlink ref="G331" r:id="rId133"/>
+    <hyperlink ref="G336" r:id="rId134"/>
+    <hyperlink ref="G356" r:id="rId135"/>
+    <hyperlink ref="G357" r:id="rId136"/>
+    <hyperlink ref="G359" r:id="rId137"/>
+    <hyperlink ref="G365" r:id="rId138"/>
+    <hyperlink ref="G373" r:id="rId139"/>
+    <hyperlink ref="G395" r:id="rId140"/>
+    <hyperlink ref="G400" r:id="rId141"/>
+    <hyperlink ref="G405" r:id="rId142"/>
+    <hyperlink ref="G409" r:id="rId143"/>
+    <hyperlink ref="G411" r:id="rId144"/>
+    <hyperlink ref="G419" r:id="rId145"/>
+    <hyperlink ref="F426" r:id="rId146"/>
+    <hyperlink ref="G429" r:id="rId147"/>
+    <hyperlink ref="G433" r:id="rId148"/>
+    <hyperlink ref="E438" r:id="rId149" location="bids-extension-proposals"/>
+    <hyperlink ref="E440" r:id="rId150"/>
+    <hyperlink ref="E441" r:id="rId151"/>
+    <hyperlink ref="E442" r:id="rId152"/>
+    <hyperlink ref="E443" r:id="rId153"/>
+    <hyperlink ref="E444" r:id="rId154"/>
+    <hyperlink ref="E445" r:id="rId155"/>
+    <hyperlink ref="E446" r:id="rId156"/>
+    <hyperlink ref="E447" r:id="rId157"/>
+    <hyperlink ref="E448" r:id="rId158"/>
+    <hyperlink ref="E449" r:id="rId159"/>
+    <hyperlink ref="E450" r:id="rId160"/>
+    <hyperlink ref="E451" r:id="rId161"/>
+    <hyperlink ref="H451" r:id="rId162"/>
+    <hyperlink ref="E452" r:id="rId163"/>
+    <hyperlink ref="E453" r:id="rId164"/>
+    <hyperlink ref="H453" r:id="rId165"/>
+    <hyperlink ref="E454" r:id="rId166"/>
+    <hyperlink ref="E455" r:id="rId167"/>
+    <hyperlink ref="E456" r:id="rId168"/>
+    <hyperlink ref="E457" r:id="rId169"/>
+    <hyperlink ref="E458" r:id="rId170"/>
+    <hyperlink ref="E459" r:id="rId171"/>
+    <hyperlink ref="E460" r:id="rId172"/>
+    <hyperlink ref="E461" r:id="rId173"/>
+    <hyperlink ref="E464" r:id="rId174"/>
+    <hyperlink ref="E465" r:id="rId175"/>
+    <hyperlink ref="E466" r:id="rId176"/>
+    <hyperlink ref="E467" r:id="rId177"/>
+    <hyperlink ref="G472" r:id="rId178"/>
+    <hyperlink ref="G473" r:id="rId179"/>
+    <hyperlink ref="E546" r:id="rId180"/>
+    <hyperlink ref="E547" r:id="rId181"/>
+    <hyperlink ref="E548" r:id="rId182"/>
+    <hyperlink ref="E549" r:id="rId183"/>
+    <hyperlink ref="E550" r:id="rId184"/>
+    <hyperlink ref="E551" r:id="rId185"/>
+    <hyperlink ref="E552" r:id="rId186"/>
+    <hyperlink ref="E553" r:id="rId187"/>
+    <hyperlink ref="E554" r:id="rId188"/>
+    <hyperlink ref="E555" r:id="rId189"/>
+    <hyperlink ref="E559" r:id="rId190"/>
+    <hyperlink ref="E560" r:id="rId191"/>
+    <hyperlink ref="E561" r:id="rId192"/>
+    <hyperlink ref="E562" r:id="rId193"/>
+    <hyperlink ref="E563" r:id="rId194"/>
+    <hyperlink ref="E564" r:id="rId195"/>
+    <hyperlink ref="E565" r:id="rId196"/>
+    <hyperlink ref="E566" r:id="rId197"/>
+    <hyperlink ref="E567" r:id="rId198"/>
+    <hyperlink ref="E568" r:id="rId199"/>
+    <hyperlink ref="E572" r:id="rId200" location="ctf"/>
+    <hyperlink ref="G572" r:id="rId201"/>
+    <hyperlink ref="E573" r:id="rId202" location="neuromagelektamegin"/>
+    <hyperlink ref="G573" r:id="rId203"/>
+    <hyperlink ref="E574" r:id="rId204" location="bti4d-neuroimaging"/>
+    <hyperlink ref="G574" r:id="rId205"/>
+    <hyperlink ref="E575" r:id="rId206" location="kityokogawaricoh"/>
+    <hyperlink ref="G575" r:id="rId207"/>
+    <hyperlink ref="E576" r:id="rId208" location="kriss"/>
+    <hyperlink ref="G576" r:id="rId209"/>
+    <hyperlink ref="E577" r:id="rId210" location="itab"/>
+    <hyperlink ref="G577" r:id="rId211"/>
+    <hyperlink ref="G583" r:id="rId212"/>
+    <hyperlink ref="G587" r:id="rId213"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
-  <pageSetup orientation="portrait"/>
   <legacyDrawing r:id="rId214"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>